<commit_message>
corrijido setores duplicados na planilha de Banco de Dados média por total de ocorrências para análise das diferenças
</commit_message>
<xml_diff>
--- a/Banco de Dados de PADS/SetoresRelevantes.xlsx
+++ b/Banco de Dados de PADS/SetoresRelevantes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>SETORES RELEVANTES GLOBAL</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>COGSA</t>
+  </si>
+  <si>
+    <t>Secretaria de Gestão de Serviços</t>
+  </si>
+  <si>
+    <t>Coordenadoria de InfraEstrutura Predial</t>
+  </si>
+  <si>
+    <t>Coordenadoria de Segurança , Transporte e Apoio Administrativo</t>
+  </si>
+  <si>
+    <t>SECRETARIA/COORDENADORIA RESP</t>
   </si>
 </sst>
 </file>
@@ -423,130 +435,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E1" sqref="E1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="50.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Banco de Dados alterado para conter todos os dados atualizados da siglas e também criado o racional para criação dos paretos na coluna Gráficos Dinamico.
</commit_message>
<xml_diff>
--- a/Banco de Dados de PADS/SetoresRelevantes.xlsx
+++ b/Banco de Dados de PADS/SetoresRelevantes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13395"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13395"/>
   </bookViews>
   <sheets>
     <sheet name="Siglas Completas(Atngias+Novas)" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>SETORES RELEVANTES GLOBAL</t>
   </si>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:C23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,9 +594,6 @@
       </c>
       <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>